<commit_message>
atualização dos passo a passos
</commit_message>
<xml_diff>
--- a/output/semivariogram-models.xlsx
+++ b/output/semivariogram-models.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -470,6 +470,72 @@
         <v>0.8323</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>2015</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Sph</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.6611</v>
+      </c>
+      <c r="E4">
+        <v>1.2411</v>
+      </c>
+      <c r="F4">
+        <v>0.21</v>
+      </c>
+      <c r="G4">
+        <v>0.5326726291193296</v>
+      </c>
+      <c r="H4">
+        <v>93880.3311</v>
+      </c>
+      <c r="I4">
+        <v>0.9224</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>2016</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Sph</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>0.7436</v>
+      </c>
+      <c r="E5">
+        <v>1.4251</v>
+      </c>
+      <c r="F5">
+        <v>0.23</v>
+      </c>
+      <c r="G5">
+        <v>0.5217879447056347</v>
+      </c>
+      <c r="H5">
+        <v>209752.6425</v>
+      </c>
+      <c r="I5">
+        <v>0.856</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>